<commit_message>
material complementar em 00_data
</commit_message>
<xml_diff>
--- a/00_data/CollectorList.xlsx
+++ b/00_data/CollectorList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\NAS_IPeC\PBC-Pesquisa\PROGRAMACAO\2022-2025\pbc_tur\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PBC-PESQUISA\PROG_LOCAL\pbc_tur\00_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82F1CC6D-71E7-4147-B5DD-D7DFBE5DD730}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52077B21-7F40-44F1-A261-A6D5F8F06185}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43200" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CollectorList" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="40">
   <si>
     <t>CollectorID</t>
   </si>
@@ -137,6 +137,9 @@
   </si>
   <si>
     <t>09/01/2024</t>
+  </si>
+  <si>
+    <t>TIRAR</t>
   </si>
 </sst>
 </file>
@@ -982,7 +985,7 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1062,6 +1065,9 @@
       <c r="G3" t="s">
         <v>30</v>
       </c>
+      <c r="H3" t="s">
+        <v>39</v>
+      </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
     </row>
@@ -1311,6 +1317,9 @@
       </c>
       <c r="G13" t="s">
         <v>30</v>
+      </c>
+      <c r="H13" t="s">
+        <v>39</v>
       </c>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>

</xml_diff>